<commit_message>
Complete upto Change Password Module
</commit_message>
<xml_diff>
--- a/src/test/java/com/guru99BankingDemo/testData/AccountModuleData.xlsx
+++ b/src/test/java/com/guru99BankingDemo/testData/AccountModuleData.xlsx
@@ -4,14 +4,16 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="23415" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="23415" windowHeight="11160" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="AddAccountData" sheetId="8" r:id="rId1"/>
     <sheet name="EditDeleteAccountNoData" sheetId="9" r:id="rId2"/>
+    <sheet name="DepositData" sheetId="10" r:id="rId3"/>
+    <sheet name="WithdrawalData" sheetId="11" r:id="rId4"/>
+    <sheet name="FundTransferData" sheetId="12" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1:S34"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="22">
   <si>
     <t>Customer Id</t>
   </si>
@@ -60,6 +62,33 @@
   </si>
   <si>
     <t>!@@##$%</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>First Deposit</t>
+  </si>
+  <si>
+    <t>fvgdfcvg</t>
+  </si>
+  <si>
+    <t>fgfgfg</t>
+  </si>
+  <si>
+    <t>!@#$%^</t>
+  </si>
+  <si>
+    <t>Payers Account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payees Account </t>
+  </si>
+  <si>
+    <t>Fund transfer</t>
   </si>
 </sst>
 </file>
@@ -128,7 +157,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
@@ -138,8 +167,12 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -157,10 +190,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -465,7 +508,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -583,7 +626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -618,4 +661,273 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="44" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="29.25" customHeight="1">
+      <c r="A1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="4">
+        <v>968754</v>
+      </c>
+      <c r="B3" s="4">
+        <v>200</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="4">
+        <v>91673</v>
+      </c>
+      <c r="B4" s="4">
+        <v>-1</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A6" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="51.5703125" customWidth="1"/>
+    <col min="3" max="3" width="41.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="4">
+        <v>968754</v>
+      </c>
+      <c r="B3" s="4">
+        <v>200</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="4">
+        <v>91673</v>
+      </c>
+      <c r="B4" s="4">
+        <v>-1</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A6" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" customWidth="1"/>
+    <col min="3" max="4" width="26.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="4">
+        <v>968754</v>
+      </c>
+      <c r="B3" s="4">
+        <v>49656548</v>
+      </c>
+      <c r="C3" s="4">
+        <v>500</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="4">
+        <v>91673</v>
+      </c>
+      <c r="B4" s="4">
+        <v>91680</v>
+      </c>
+      <c r="C4" s="4">
+        <v>-1</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A6" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2"/>
+    <hyperlink ref="C6" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
All ModuleAutomation test Complete
</commit_message>
<xml_diff>
--- a/src/test/java/com/guru99BankingDemo/testData/AccountModuleData.xlsx
+++ b/src/test/java/com/guru99BankingDemo/testData/AccountModuleData.xlsx
@@ -4,14 +4,16 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="23415" windowHeight="11160" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="23415" windowHeight="11160" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="AddAccountData" sheetId="8" r:id="rId1"/>
-    <sheet name="EditDeleteAccountNoData" sheetId="9" r:id="rId2"/>
+    <sheet name="EditDeleteEnquiryStatementData" sheetId="9" r:id="rId2"/>
     <sheet name="DepositData" sheetId="10" r:id="rId3"/>
     <sheet name="WithdrawalData" sheetId="11" r:id="rId4"/>
     <sheet name="FundTransferData" sheetId="12" r:id="rId5"/>
+    <sheet name="ChangePasswordData" sheetId="13" r:id="rId6"/>
+    <sheet name="CustomisedStatementData" sheetId="14" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="41">
   <si>
     <t>Customer Id</t>
   </si>
@@ -89,6 +91,63 @@
   </si>
   <si>
     <t>Fund transfer</t>
+  </si>
+  <si>
+    <t>Old Password</t>
+  </si>
+  <si>
+    <t>New Password</t>
+  </si>
+  <si>
+    <t>Confirm Password</t>
+  </si>
+  <si>
+    <t>123@123</t>
+  </si>
+  <si>
+    <t>113@113</t>
+  </si>
+  <si>
+    <t>112#112</t>
+  </si>
+  <si>
+    <t>467915!@</t>
+  </si>
+  <si>
+    <t>From Month</t>
+  </si>
+  <si>
+    <t>From Day</t>
+  </si>
+  <si>
+    <t>From Year</t>
+  </si>
+  <si>
+    <t>To Month</t>
+  </si>
+  <si>
+    <t>To Day</t>
+  </si>
+  <si>
+    <t>To Year</t>
+  </si>
+  <si>
+    <t>Minimun Transaction</t>
+  </si>
+  <si>
+    <t>Number Of Transaction</t>
+  </si>
+  <si>
+    <t>sffderfdef</t>
+  </si>
+  <si>
+    <t>dggfdgd</t>
+  </si>
+  <si>
+    <t>dfdfdfdf</t>
+  </si>
+  <si>
+    <t>!!@##%%</t>
   </si>
 </sst>
 </file>
@@ -172,7 +231,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -198,6 +257,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -508,7 +573,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -524,9 +589,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="48.42578125" customWidth="1"/>
-    <col min="2" max="2" width="38.5703125" customWidth="1"/>
-    <col min="3" max="3" width="70.140625" customWidth="1"/>
+    <col min="1" max="1" width="48.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="38.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="70.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -627,12 +692,12 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="56.42578125" customWidth="1"/>
+    <col min="1" max="1" width="56.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="27.75" customHeight="1">
@@ -673,9 +738,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="39.85546875" customWidth="1"/>
-    <col min="3" max="3" width="44" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="44" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="29.25" customHeight="1">
@@ -757,9 +822,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
-    <col min="2" max="2" width="51.5703125" customWidth="1"/>
-    <col min="3" max="3" width="41.7109375" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="51.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="41.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -835,15 +900,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="32" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" customWidth="1"/>
-    <col min="3" max="4" width="26.85546875" customWidth="1"/>
+    <col min="1" max="1" width="32" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="26.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -930,4 +995,265 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="40.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="50" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="50.85546875" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="33" customHeight="1">
+      <c r="A1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="10">
+        <v>12345678</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="10">
+        <v>12345</v>
+      </c>
+      <c r="C4" s="10">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="8" max="8" width="28.140625" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="25.5" customHeight="1">
+      <c r="A1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="4">
+        <v>96584564</v>
+      </c>
+      <c r="B2" s="4">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4">
+        <v>20</v>
+      </c>
+      <c r="D2" s="4">
+        <v>2021</v>
+      </c>
+      <c r="E2" s="4">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4">
+        <v>21</v>
+      </c>
+      <c r="G2" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H2" s="4">
+        <v>500</v>
+      </c>
+      <c r="I2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="4">
+        <v>91673</v>
+      </c>
+      <c r="B3" s="4">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4">
+        <v>21</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2021</v>
+      </c>
+      <c r="E3" s="4">
+        <v>4</v>
+      </c>
+      <c r="F3" s="4">
+        <v>20</v>
+      </c>
+      <c r="G3" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H3" s="4">
+        <v>500</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="4">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4">
+        <v>20</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2021</v>
+      </c>
+      <c r="E5" s="4">
+        <v>4</v>
+      </c>
+      <c r="F5" s="4">
+        <v>21</v>
+      </c>
+      <c r="G5" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2020</v>
+      </c>
+      <c r="E6" s="4">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4">
+        <v>5</v>
+      </c>
+      <c r="G6" s="4">
+        <v>2021</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A6" r:id="rId1"/>
+    <hyperlink ref="H6" r:id="rId2"/>
+    <hyperlink ref="I6" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>